<commit_message>
Bổ sung cột Mô tả và giải pháp chi tiết hơn
</commit_message>
<xml_diff>
--- a/01_Document/Phân tích yêu cầu/Peer review/[PeerReview]1412405_Review_1412356.xlsx
+++ b/01_Document/Phân tích yêu cầu/Peer review/[PeerReview]1412405_Review_1412356.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QLXeKhach-C43\01_Document\Phân tích yêu cầu\Peer review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HONG PHUC\Desktop\QLXeKhach-C43\01_Document\Phân tích yêu cầu\Peer review\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1597,12 +1597,6 @@
     <t>Mục 3.2.3</t>
   </si>
   <si>
-    <t>Chỉnh lại thành "Ban giám đốc"</t>
-  </si>
-  <si>
-    <t>Ghi nhầm mô tả: "Ban quản lí"</t>
-  </si>
-  <si>
     <t>Thảo Nguyên</t>
   </si>
   <si>
@@ -1610,9 +1604,6 @@
   </si>
   <si>
     <t>Chưa ghi rõ thông tin khảo sát</t>
-  </si>
-  <si>
-    <t>Bổ sung nội dung chi tiết thông tin khảo sát</t>
   </si>
   <si>
     <t>Mục 3.2.2</t>
@@ -1642,9 +1633,6 @@
     <t>"Thiết lập đường đi mới" chưa đủ ý nghĩa so với đặc tả</t>
   </si>
   <si>
-    <t xml:space="preserve">Thay thế bằng " Thiết lập các tuyến đường mới" </t>
-  </si>
-  <si>
     <t xml:space="preserve">Thừa tác viên bị dư thừa "Ban giám đốc: Thông tin trạm" </t>
   </si>
   <si>
@@ -1654,7 +1642,19 @@
     <t>Thiếu thực thể nghiệp vụ</t>
   </si>
   <si>
-    <t>Bổ sung thực thể nghiệp vụ</t>
+    <t>Bổ sung nội dung chi tiết thông tin khảo sát: chi phí, tỉ lệ đón khách tiềm năng, số km</t>
+  </si>
+  <si>
+    <t>Ghi nhầm mô tả: "UC bắt đầu khi ban quản lí kiến nghị dừng hoạt động tuyến xe vì doanh thu đem lại quá thấp"</t>
+  </si>
+  <si>
+    <t>Chỉnh lại thành "UC bắt đầu khi ban giám đốc kiến nghị dừng hoạt động tuyến xe vì doanh thu đem lại quá thấp"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thay thế bằng " Thiết lập các tuyến đường đi mới" </t>
+  </si>
+  <si>
+    <t>Bổ sung thực thể nghiệp vụ: thông tin tuyến</t>
   </si>
 </sst>
 </file>
@@ -4229,49 +4229,57 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="171" fontId="23" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="23" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="171" fontId="23" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -4338,14 +4346,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -18950,7 +18950,7 @@
   <dimension ref="A1:AN82"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31:D32"/>
+      <selection activeCell="Q33" sqref="Q33:V33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19027,7 +19027,7 @@
       <c r="R2" s="463"/>
       <c r="S2" s="464"/>
       <c r="T2" s="473" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="U2" s="474"/>
       <c r="V2" s="474"/>
@@ -19211,7 +19211,7 @@
       <c r="R8" s="471"/>
       <c r="S8" s="472"/>
       <c r="T8" s="484" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="U8" s="485"/>
       <c r="V8" s="486"/>
@@ -19380,7 +19380,7 @@
       <c r="D15" s="517"/>
       <c r="E15" s="518"/>
       <c r="F15" s="519" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="G15" s="519"/>
       <c r="H15" s="519"/>
@@ -19453,7 +19453,7 @@
       </c>
       <c r="G17" s="525"/>
       <c r="H17" s="536" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="I17" s="526"/>
       <c r="J17" s="526"/>
@@ -19465,7 +19465,7 @@
       <c r="P17" s="526"/>
       <c r="Q17" s="537"/>
       <c r="R17" s="538" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="S17" s="538"/>
       <c r="T17" s="538"/>
@@ -19498,7 +19498,7 @@
       </c>
       <c r="K18" s="546"/>
       <c r="L18" s="545" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="M18" s="545"/>
       <c r="N18" s="547" t="s">
@@ -19827,14 +19827,14 @@
       <c r="C28" s="573" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="607" t="s">
-        <v>306</v>
+      <c r="D28" s="574" t="s">
+        <v>303</v>
       </c>
       <c r="E28" s="575" t="s">
         <v>298</v>
       </c>
       <c r="F28" s="576" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G28" s="577"/>
       <c r="H28" s="577"/>
@@ -19848,14 +19848,14 @@
         <v>256</v>
       </c>
       <c r="N28" s="565" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="O28" s="581" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="P28" s="582"/>
       <c r="Q28" s="583" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="R28" s="584"/>
       <c r="S28" s="584"/>
@@ -19873,12 +19873,12 @@
       <c r="C29" s="573" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="608"/>
+      <c r="D29" s="586"/>
       <c r="E29" s="575" t="s">
         <v>298</v>
       </c>
       <c r="F29" s="576" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G29" s="577"/>
       <c r="H29" s="577"/>
@@ -19892,14 +19892,14 @@
         <v>256</v>
       </c>
       <c r="N29" s="565" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="O29" s="581" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="P29" s="582"/>
       <c r="Q29" s="583" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="R29" s="584"/>
       <c r="S29" s="584"/>
@@ -19917,14 +19917,14 @@
       <c r="C30" s="573" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="574" t="s">
+      <c r="D30" s="587" t="s">
         <v>299</v>
       </c>
       <c r="E30" s="575" t="s">
         <v>298</v>
       </c>
       <c r="F30" s="576" t="s">
-        <v>301</v>
+        <v>316</v>
       </c>
       <c r="G30" s="577"/>
       <c r="H30" s="577"/>
@@ -19938,14 +19938,14 @@
         <v>256</v>
       </c>
       <c r="N30" s="565" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="O30" s="581" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="P30" s="582"/>
       <c r="Q30" s="583" t="s">
-        <v>300</v>
+        <v>317</v>
       </c>
       <c r="R30" s="584"/>
       <c r="S30" s="584"/>
@@ -19963,14 +19963,14 @@
       <c r="C31" s="573" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="607" t="s">
-        <v>313</v>
+      <c r="D31" s="574" t="s">
+        <v>310</v>
       </c>
       <c r="E31" s="575" t="s">
         <v>298</v>
       </c>
       <c r="F31" s="576" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G31" s="577"/>
       <c r="H31" s="577"/>
@@ -19984,14 +19984,14 @@
         <v>256</v>
       </c>
       <c r="N31" s="565" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="O31" s="581" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="P31" s="582"/>
       <c r="Q31" s="583" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="R31" s="584"/>
       <c r="S31" s="584"/>
@@ -20009,12 +20009,12 @@
       <c r="C32" s="573" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="608"/>
+      <c r="D32" s="586"/>
       <c r="E32" s="575" t="s">
         <v>298</v>
       </c>
       <c r="F32" s="576" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="G32" s="577"/>
       <c r="H32" s="577"/>
@@ -20028,14 +20028,14 @@
         <v>256</v>
       </c>
       <c r="N32" s="565" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="O32" s="581" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="P32" s="582"/>
       <c r="Q32" s="583" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="R32" s="584"/>
       <c r="S32" s="584"/>
@@ -20053,14 +20053,14 @@
       <c r="C33" s="573" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="574" t="s">
-        <v>313</v>
+      <c r="D33" s="587" t="s">
+        <v>310</v>
       </c>
       <c r="E33" s="575" t="s">
         <v>298</v>
       </c>
       <c r="F33" s="576" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="G33" s="577"/>
       <c r="H33" s="577"/>
@@ -20074,10 +20074,10 @@
         <v>256</v>
       </c>
       <c r="N33" s="565" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="O33" s="581" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="P33" s="582"/>
       <c r="Q33" s="583" t="s">
@@ -20099,29 +20099,29 @@
       <c r="C34" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="574"/>
+      <c r="D34" s="587"/>
       <c r="E34" s="575"/>
-      <c r="F34" s="586"/>
-      <c r="G34" s="587"/>
-      <c r="H34" s="587"/>
-      <c r="I34" s="587"/>
-      <c r="J34" s="587"/>
-      <c r="K34" s="587"/>
-      <c r="L34" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M34" s="589" t="s">
+      <c r="F34" s="588"/>
+      <c r="G34" s="589"/>
+      <c r="H34" s="589"/>
+      <c r="I34" s="589"/>
+      <c r="J34" s="589"/>
+      <c r="K34" s="589"/>
+      <c r="L34" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M34" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N34" s="565"/>
       <c r="O34" s="581"/>
       <c r="P34" s="582"/>
-      <c r="Q34" s="590"/>
-      <c r="R34" s="591"/>
-      <c r="S34" s="591"/>
-      <c r="T34" s="591"/>
-      <c r="U34" s="591"/>
-      <c r="V34" s="592"/>
+      <c r="Q34" s="592"/>
+      <c r="R34" s="593"/>
+      <c r="S34" s="593"/>
+      <c r="T34" s="593"/>
+      <c r="U34" s="593"/>
+      <c r="V34" s="594"/>
       <c r="W34" s="565"/>
       <c r="X34" s="566"/>
       <c r="Y34" s="567"/>
@@ -20133,29 +20133,29 @@
       <c r="C35" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D35" s="574"/>
+      <c r="D35" s="587"/>
       <c r="E35" s="575"/>
-      <c r="F35" s="586"/>
-      <c r="G35" s="587"/>
-      <c r="H35" s="587"/>
-      <c r="I35" s="587"/>
-      <c r="J35" s="587"/>
-      <c r="K35" s="587"/>
-      <c r="L35" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M35" s="589" t="s">
+      <c r="F35" s="588"/>
+      <c r="G35" s="589"/>
+      <c r="H35" s="589"/>
+      <c r="I35" s="589"/>
+      <c r="J35" s="589"/>
+      <c r="K35" s="589"/>
+      <c r="L35" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M35" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N35" s="565"/>
       <c r="O35" s="581"/>
       <c r="P35" s="582"/>
-      <c r="Q35" s="590"/>
-      <c r="R35" s="591"/>
-      <c r="S35" s="591"/>
-      <c r="T35" s="591"/>
-      <c r="U35" s="591"/>
-      <c r="V35" s="592"/>
+      <c r="Q35" s="592"/>
+      <c r="R35" s="593"/>
+      <c r="S35" s="593"/>
+      <c r="T35" s="593"/>
+      <c r="U35" s="593"/>
+      <c r="V35" s="594"/>
       <c r="W35" s="565"/>
       <c r="X35" s="566"/>
       <c r="Y35" s="567"/>
@@ -20168,29 +20168,29 @@
       <c r="C36" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="574"/>
+      <c r="D36" s="587"/>
       <c r="E36" s="575"/>
-      <c r="F36" s="586"/>
-      <c r="G36" s="587"/>
-      <c r="H36" s="587"/>
-      <c r="I36" s="587"/>
-      <c r="J36" s="587"/>
-      <c r="K36" s="587"/>
-      <c r="L36" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M36" s="589" t="s">
+      <c r="F36" s="588"/>
+      <c r="G36" s="589"/>
+      <c r="H36" s="589"/>
+      <c r="I36" s="589"/>
+      <c r="J36" s="589"/>
+      <c r="K36" s="589"/>
+      <c r="L36" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M36" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N36" s="565"/>
       <c r="O36" s="581"/>
       <c r="P36" s="582"/>
-      <c r="Q36" s="590"/>
-      <c r="R36" s="591"/>
-      <c r="S36" s="591"/>
-      <c r="T36" s="591"/>
-      <c r="U36" s="591"/>
-      <c r="V36" s="592"/>
+      <c r="Q36" s="592"/>
+      <c r="R36" s="593"/>
+      <c r="S36" s="593"/>
+      <c r="T36" s="593"/>
+      <c r="U36" s="593"/>
+      <c r="V36" s="594"/>
       <c r="W36" s="565"/>
       <c r="X36" s="566"/>
       <c r="Y36" s="567"/>
@@ -20204,29 +20204,29 @@
       <c r="C37" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="574"/>
+      <c r="D37" s="587"/>
       <c r="E37" s="575"/>
-      <c r="F37" s="586"/>
-      <c r="G37" s="587"/>
-      <c r="H37" s="587"/>
-      <c r="I37" s="587"/>
-      <c r="J37" s="587"/>
-      <c r="K37" s="587"/>
-      <c r="L37" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M37" s="589" t="s">
+      <c r="F37" s="588"/>
+      <c r="G37" s="589"/>
+      <c r="H37" s="589"/>
+      <c r="I37" s="589"/>
+      <c r="J37" s="589"/>
+      <c r="K37" s="589"/>
+      <c r="L37" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M37" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N37" s="565"/>
       <c r="O37" s="581"/>
       <c r="P37" s="582"/>
-      <c r="Q37" s="590"/>
-      <c r="R37" s="591"/>
-      <c r="S37" s="591"/>
-      <c r="T37" s="591"/>
-      <c r="U37" s="591"/>
-      <c r="V37" s="592"/>
+      <c r="Q37" s="592"/>
+      <c r="R37" s="593"/>
+      <c r="S37" s="593"/>
+      <c r="T37" s="593"/>
+      <c r="U37" s="593"/>
+      <c r="V37" s="594"/>
       <c r="W37" s="565"/>
       <c r="X37" s="566"/>
       <c r="Y37" s="567"/>
@@ -20240,275 +20240,275 @@
       <c r="C38" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="574"/>
+      <c r="D38" s="587"/>
       <c r="E38" s="575"/>
-      <c r="F38" s="586"/>
-      <c r="G38" s="587"/>
-      <c r="H38" s="587"/>
-      <c r="I38" s="587"/>
-      <c r="J38" s="587"/>
-      <c r="K38" s="587"/>
-      <c r="L38" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M38" s="589" t="s">
+      <c r="F38" s="588"/>
+      <c r="G38" s="589"/>
+      <c r="H38" s="589"/>
+      <c r="I38" s="589"/>
+      <c r="J38" s="589"/>
+      <c r="K38" s="589"/>
+      <c r="L38" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M38" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N38" s="565"/>
       <c r="O38" s="581"/>
       <c r="P38" s="582"/>
-      <c r="Q38" s="590"/>
-      <c r="R38" s="591"/>
-      <c r="S38" s="591"/>
-      <c r="T38" s="591"/>
-      <c r="U38" s="591"/>
-      <c r="V38" s="592"/>
+      <c r="Q38" s="592"/>
+      <c r="R38" s="593"/>
+      <c r="S38" s="593"/>
+      <c r="T38" s="593"/>
+      <c r="U38" s="593"/>
+      <c r="V38" s="594"/>
       <c r="W38" s="565"/>
       <c r="X38" s="566"/>
       <c r="Y38" s="567"/>
       <c r="Z38" s="465"/>
     </row>
-    <row r="39" spans="1:26" s="594" customFormat="1" ht="42" customHeight="1">
-      <c r="A39" s="593"/>
+    <row r="39" spans="1:26" s="596" customFormat="1" ht="42" customHeight="1">
+      <c r="A39" s="595"/>
       <c r="B39" s="572">
         <v>13</v>
       </c>
       <c r="C39" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D39" s="574"/>
+      <c r="D39" s="587"/>
       <c r="E39" s="575"/>
-      <c r="F39" s="586"/>
-      <c r="G39" s="587"/>
-      <c r="H39" s="587"/>
-      <c r="I39" s="587"/>
-      <c r="J39" s="587"/>
-      <c r="K39" s="587"/>
-      <c r="L39" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M39" s="589" t="s">
+      <c r="F39" s="588"/>
+      <c r="G39" s="589"/>
+      <c r="H39" s="589"/>
+      <c r="I39" s="589"/>
+      <c r="J39" s="589"/>
+      <c r="K39" s="589"/>
+      <c r="L39" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M39" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N39" s="565"/>
       <c r="O39" s="581"/>
       <c r="P39" s="582"/>
-      <c r="Q39" s="590"/>
-      <c r="R39" s="591"/>
-      <c r="S39" s="591"/>
-      <c r="T39" s="591"/>
-      <c r="U39" s="591"/>
-      <c r="V39" s="592"/>
+      <c r="Q39" s="592"/>
+      <c r="R39" s="593"/>
+      <c r="S39" s="593"/>
+      <c r="T39" s="593"/>
+      <c r="U39" s="593"/>
+      <c r="V39" s="594"/>
       <c r="W39" s="565"/>
       <c r="X39" s="566"/>
       <c r="Y39" s="567"/>
     </row>
-    <row r="40" spans="1:26" s="594" customFormat="1" ht="42" customHeight="1">
-      <c r="A40" s="593"/>
+    <row r="40" spans="1:26" s="596" customFormat="1" ht="42" customHeight="1">
+      <c r="A40" s="595"/>
       <c r="B40" s="572">
         <v>14</v>
       </c>
       <c r="C40" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D40" s="574"/>
+      <c r="D40" s="587"/>
       <c r="E40" s="575"/>
-      <c r="F40" s="586"/>
-      <c r="G40" s="587"/>
-      <c r="H40" s="587"/>
-      <c r="I40" s="587"/>
-      <c r="J40" s="587"/>
-      <c r="K40" s="587"/>
-      <c r="L40" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M40" s="589" t="s">
+      <c r="F40" s="588"/>
+      <c r="G40" s="589"/>
+      <c r="H40" s="589"/>
+      <c r="I40" s="589"/>
+      <c r="J40" s="589"/>
+      <c r="K40" s="589"/>
+      <c r="L40" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M40" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N40" s="565"/>
       <c r="O40" s="581"/>
       <c r="P40" s="582"/>
-      <c r="Q40" s="590"/>
-      <c r="R40" s="591"/>
-      <c r="S40" s="591"/>
-      <c r="T40" s="591"/>
-      <c r="U40" s="591"/>
-      <c r="V40" s="592"/>
+      <c r="Q40" s="592"/>
+      <c r="R40" s="593"/>
+      <c r="S40" s="593"/>
+      <c r="T40" s="593"/>
+      <c r="U40" s="593"/>
+      <c r="V40" s="594"/>
       <c r="W40" s="565"/>
       <c r="X40" s="566"/>
       <c r="Y40" s="567"/>
     </row>
-    <row r="41" spans="1:26" s="594" customFormat="1" ht="42" customHeight="1">
-      <c r="A41" s="593"/>
+    <row r="41" spans="1:26" s="596" customFormat="1" ht="42" customHeight="1">
+      <c r="A41" s="595"/>
       <c r="B41" s="572">
         <v>15</v>
       </c>
       <c r="C41" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D41" s="574"/>
+      <c r="D41" s="587"/>
       <c r="E41" s="575"/>
-      <c r="F41" s="586"/>
-      <c r="G41" s="587"/>
-      <c r="H41" s="587"/>
-      <c r="I41" s="587"/>
-      <c r="J41" s="587"/>
-      <c r="K41" s="587"/>
-      <c r="L41" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M41" s="589" t="s">
+      <c r="F41" s="588"/>
+      <c r="G41" s="589"/>
+      <c r="H41" s="589"/>
+      <c r="I41" s="589"/>
+      <c r="J41" s="589"/>
+      <c r="K41" s="589"/>
+      <c r="L41" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M41" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N41" s="565"/>
       <c r="O41" s="581"/>
       <c r="P41" s="582"/>
-      <c r="Q41" s="590"/>
-      <c r="R41" s="591"/>
-      <c r="S41" s="591"/>
-      <c r="T41" s="591"/>
-      <c r="U41" s="591"/>
-      <c r="V41" s="592"/>
+      <c r="Q41" s="592"/>
+      <c r="R41" s="593"/>
+      <c r="S41" s="593"/>
+      <c r="T41" s="593"/>
+      <c r="U41" s="593"/>
+      <c r="V41" s="594"/>
       <c r="W41" s="565"/>
       <c r="X41" s="566"/>
       <c r="Y41" s="567"/>
     </row>
-    <row r="42" spans="1:26" s="594" customFormat="1" ht="42" customHeight="1">
-      <c r="A42" s="593"/>
+    <row r="42" spans="1:26" s="596" customFormat="1" ht="42" customHeight="1">
+      <c r="A42" s="595"/>
       <c r="B42" s="572">
         <v>16</v>
       </c>
       <c r="C42" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D42" s="574"/>
+      <c r="D42" s="587"/>
       <c r="E42" s="575"/>
-      <c r="F42" s="586"/>
-      <c r="G42" s="587"/>
-      <c r="H42" s="587"/>
-      <c r="I42" s="587"/>
-      <c r="J42" s="587"/>
-      <c r="K42" s="587"/>
-      <c r="L42" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M42" s="589" t="s">
+      <c r="F42" s="588"/>
+      <c r="G42" s="589"/>
+      <c r="H42" s="589"/>
+      <c r="I42" s="589"/>
+      <c r="J42" s="589"/>
+      <c r="K42" s="589"/>
+      <c r="L42" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M42" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N42" s="565"/>
       <c r="O42" s="581"/>
       <c r="P42" s="582"/>
-      <c r="Q42" s="590"/>
-      <c r="R42" s="591"/>
-      <c r="S42" s="591"/>
-      <c r="T42" s="591"/>
-      <c r="U42" s="591"/>
-      <c r="V42" s="592"/>
+      <c r="Q42" s="592"/>
+      <c r="R42" s="593"/>
+      <c r="S42" s="593"/>
+      <c r="T42" s="593"/>
+      <c r="U42" s="593"/>
+      <c r="V42" s="594"/>
       <c r="W42" s="565"/>
       <c r="X42" s="566"/>
       <c r="Y42" s="567"/>
     </row>
-    <row r="43" spans="1:26" s="594" customFormat="1" ht="42" customHeight="1">
-      <c r="A43" s="593"/>
+    <row r="43" spans="1:26" s="596" customFormat="1" ht="42" customHeight="1">
+      <c r="A43" s="595"/>
       <c r="B43" s="572">
         <v>17</v>
       </c>
       <c r="C43" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D43" s="574"/>
+      <c r="D43" s="587"/>
       <c r="E43" s="575"/>
-      <c r="F43" s="586"/>
-      <c r="G43" s="587"/>
-      <c r="H43" s="587"/>
-      <c r="I43" s="587"/>
-      <c r="J43" s="587"/>
-      <c r="K43" s="587"/>
-      <c r="L43" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M43" s="589" t="s">
+      <c r="F43" s="588"/>
+      <c r="G43" s="589"/>
+      <c r="H43" s="589"/>
+      <c r="I43" s="589"/>
+      <c r="J43" s="589"/>
+      <c r="K43" s="589"/>
+      <c r="L43" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M43" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N43" s="565"/>
       <c r="O43" s="581"/>
       <c r="P43" s="582"/>
-      <c r="Q43" s="590"/>
-      <c r="R43" s="591"/>
-      <c r="S43" s="591"/>
-      <c r="T43" s="591"/>
-      <c r="U43" s="591"/>
-      <c r="V43" s="592"/>
+      <c r="Q43" s="592"/>
+      <c r="R43" s="593"/>
+      <c r="S43" s="593"/>
+      <c r="T43" s="593"/>
+      <c r="U43" s="593"/>
+      <c r="V43" s="594"/>
       <c r="W43" s="565"/>
       <c r="X43" s="566"/>
       <c r="Y43" s="567"/>
     </row>
-    <row r="44" spans="1:26" s="594" customFormat="1" ht="42" customHeight="1">
-      <c r="A44" s="593"/>
+    <row r="44" spans="1:26" s="596" customFormat="1" ht="42" customHeight="1">
+      <c r="A44" s="595"/>
       <c r="B44" s="572">
         <v>18</v>
       </c>
       <c r="C44" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D44" s="574"/>
+      <c r="D44" s="587"/>
       <c r="E44" s="575"/>
-      <c r="F44" s="586"/>
-      <c r="G44" s="587"/>
-      <c r="H44" s="587"/>
-      <c r="I44" s="587"/>
-      <c r="J44" s="587"/>
-      <c r="K44" s="587"/>
-      <c r="L44" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M44" s="589" t="s">
+      <c r="F44" s="588"/>
+      <c r="G44" s="589"/>
+      <c r="H44" s="589"/>
+      <c r="I44" s="589"/>
+      <c r="J44" s="589"/>
+      <c r="K44" s="589"/>
+      <c r="L44" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M44" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N44" s="565"/>
       <c r="O44" s="581"/>
       <c r="P44" s="582"/>
-      <c r="Q44" s="590"/>
-      <c r="R44" s="591"/>
-      <c r="S44" s="591"/>
-      <c r="T44" s="591"/>
-      <c r="U44" s="591"/>
-      <c r="V44" s="592"/>
+      <c r="Q44" s="592"/>
+      <c r="R44" s="593"/>
+      <c r="S44" s="593"/>
+      <c r="T44" s="593"/>
+      <c r="U44" s="593"/>
+      <c r="V44" s="594"/>
       <c r="W44" s="565"/>
       <c r="X44" s="566"/>
       <c r="Y44" s="567"/>
     </row>
-    <row r="45" spans="1:26" s="594" customFormat="1" ht="42" customHeight="1">
-      <c r="A45" s="593"/>
+    <row r="45" spans="1:26" s="596" customFormat="1" ht="42" customHeight="1">
+      <c r="A45" s="595"/>
       <c r="B45" s="572">
         <v>19</v>
       </c>
       <c r="C45" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D45" s="574"/>
+      <c r="D45" s="587"/>
       <c r="E45" s="575"/>
-      <c r="F45" s="586"/>
-      <c r="G45" s="587"/>
-      <c r="H45" s="587"/>
-      <c r="I45" s="587"/>
-      <c r="J45" s="587"/>
-      <c r="K45" s="587"/>
-      <c r="L45" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M45" s="589" t="s">
+      <c r="F45" s="588"/>
+      <c r="G45" s="589"/>
+      <c r="H45" s="589"/>
+      <c r="I45" s="589"/>
+      <c r="J45" s="589"/>
+      <c r="K45" s="589"/>
+      <c r="L45" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M45" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N45" s="565"/>
       <c r="O45" s="581"/>
       <c r="P45" s="582"/>
-      <c r="Q45" s="590"/>
-      <c r="R45" s="591"/>
-      <c r="S45" s="591"/>
-      <c r="T45" s="591"/>
-      <c r="U45" s="591"/>
-      <c r="V45" s="592"/>
+      <c r="Q45" s="592"/>
+      <c r="R45" s="593"/>
+      <c r="S45" s="593"/>
+      <c r="T45" s="593"/>
+      <c r="U45" s="593"/>
+      <c r="V45" s="594"/>
       <c r="W45" s="565"/>
       <c r="X45" s="566"/>
       <c r="Y45" s="567"/>
@@ -20520,29 +20520,29 @@
       <c r="C46" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D46" s="574"/>
+      <c r="D46" s="587"/>
       <c r="E46" s="575"/>
-      <c r="F46" s="586"/>
-      <c r="G46" s="587"/>
-      <c r="H46" s="587"/>
-      <c r="I46" s="587"/>
-      <c r="J46" s="587"/>
-      <c r="K46" s="587"/>
-      <c r="L46" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M46" s="589" t="s">
+      <c r="F46" s="588"/>
+      <c r="G46" s="589"/>
+      <c r="H46" s="589"/>
+      <c r="I46" s="589"/>
+      <c r="J46" s="589"/>
+      <c r="K46" s="589"/>
+      <c r="L46" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M46" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N46" s="565"/>
       <c r="O46" s="581"/>
       <c r="P46" s="582"/>
-      <c r="Q46" s="590"/>
-      <c r="R46" s="591"/>
-      <c r="S46" s="591"/>
-      <c r="T46" s="591"/>
-      <c r="U46" s="591"/>
-      <c r="V46" s="592"/>
+      <c r="Q46" s="592"/>
+      <c r="R46" s="593"/>
+      <c r="S46" s="593"/>
+      <c r="T46" s="593"/>
+      <c r="U46" s="593"/>
+      <c r="V46" s="594"/>
       <c r="W46" s="565"/>
       <c r="X46" s="566"/>
       <c r="Y46" s="567"/>
@@ -20554,29 +20554,29 @@
       <c r="C47" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D47" s="574"/>
+      <c r="D47" s="587"/>
       <c r="E47" s="575"/>
-      <c r="F47" s="586"/>
-      <c r="G47" s="587"/>
-      <c r="H47" s="587"/>
-      <c r="I47" s="587"/>
-      <c r="J47" s="587"/>
-      <c r="K47" s="587"/>
-      <c r="L47" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M47" s="589" t="s">
+      <c r="F47" s="588"/>
+      <c r="G47" s="589"/>
+      <c r="H47" s="589"/>
+      <c r="I47" s="589"/>
+      <c r="J47" s="589"/>
+      <c r="K47" s="589"/>
+      <c r="L47" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M47" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N47" s="565"/>
       <c r="O47" s="581"/>
       <c r="P47" s="582"/>
-      <c r="Q47" s="590"/>
-      <c r="R47" s="591"/>
-      <c r="S47" s="591"/>
-      <c r="T47" s="591"/>
-      <c r="U47" s="591"/>
-      <c r="V47" s="592"/>
+      <c r="Q47" s="592"/>
+      <c r="R47" s="593"/>
+      <c r="S47" s="593"/>
+      <c r="T47" s="593"/>
+      <c r="U47" s="593"/>
+      <c r="V47" s="594"/>
       <c r="W47" s="565"/>
       <c r="X47" s="566"/>
       <c r="Y47" s="567"/>
@@ -20588,29 +20588,29 @@
       <c r="C48" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D48" s="574"/>
+      <c r="D48" s="587"/>
       <c r="E48" s="575"/>
-      <c r="F48" s="586"/>
-      <c r="G48" s="587"/>
-      <c r="H48" s="587"/>
-      <c r="I48" s="587"/>
-      <c r="J48" s="587"/>
-      <c r="K48" s="587"/>
-      <c r="L48" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M48" s="589" t="s">
+      <c r="F48" s="588"/>
+      <c r="G48" s="589"/>
+      <c r="H48" s="589"/>
+      <c r="I48" s="589"/>
+      <c r="J48" s="589"/>
+      <c r="K48" s="589"/>
+      <c r="L48" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M48" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N48" s="565"/>
       <c r="O48" s="581"/>
       <c r="P48" s="582"/>
-      <c r="Q48" s="590"/>
-      <c r="R48" s="591"/>
-      <c r="S48" s="591"/>
-      <c r="T48" s="591"/>
-      <c r="U48" s="591"/>
-      <c r="V48" s="592"/>
+      <c r="Q48" s="592"/>
+      <c r="R48" s="593"/>
+      <c r="S48" s="593"/>
+      <c r="T48" s="593"/>
+      <c r="U48" s="593"/>
+      <c r="V48" s="594"/>
       <c r="W48" s="565"/>
       <c r="X48" s="566"/>
       <c r="Y48" s="567"/>
@@ -20622,29 +20622,29 @@
       <c r="C49" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D49" s="574"/>
+      <c r="D49" s="587"/>
       <c r="E49" s="575"/>
-      <c r="F49" s="586"/>
-      <c r="G49" s="587"/>
-      <c r="H49" s="587"/>
-      <c r="I49" s="587"/>
-      <c r="J49" s="587"/>
-      <c r="K49" s="587"/>
-      <c r="L49" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M49" s="589" t="s">
+      <c r="F49" s="588"/>
+      <c r="G49" s="589"/>
+      <c r="H49" s="589"/>
+      <c r="I49" s="589"/>
+      <c r="J49" s="589"/>
+      <c r="K49" s="589"/>
+      <c r="L49" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M49" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N49" s="565"/>
       <c r="O49" s="581"/>
       <c r="P49" s="582"/>
-      <c r="Q49" s="590"/>
-      <c r="R49" s="591"/>
-      <c r="S49" s="591"/>
-      <c r="T49" s="591"/>
-      <c r="U49" s="591"/>
-      <c r="V49" s="592"/>
+      <c r="Q49" s="592"/>
+      <c r="R49" s="593"/>
+      <c r="S49" s="593"/>
+      <c r="T49" s="593"/>
+      <c r="U49" s="593"/>
+      <c r="V49" s="594"/>
       <c r="W49" s="565"/>
       <c r="X49" s="566"/>
       <c r="Y49" s="567"/>
@@ -20656,29 +20656,29 @@
       <c r="C50" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D50" s="574"/>
+      <c r="D50" s="587"/>
       <c r="E50" s="575"/>
-      <c r="F50" s="586"/>
-      <c r="G50" s="587"/>
-      <c r="H50" s="587"/>
-      <c r="I50" s="587"/>
-      <c r="J50" s="587"/>
-      <c r="K50" s="587"/>
-      <c r="L50" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M50" s="589" t="s">
+      <c r="F50" s="588"/>
+      <c r="G50" s="589"/>
+      <c r="H50" s="589"/>
+      <c r="I50" s="589"/>
+      <c r="J50" s="589"/>
+      <c r="K50" s="589"/>
+      <c r="L50" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M50" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N50" s="565"/>
       <c r="O50" s="581"/>
       <c r="P50" s="582"/>
-      <c r="Q50" s="590"/>
-      <c r="R50" s="591"/>
-      <c r="S50" s="591"/>
-      <c r="T50" s="591"/>
-      <c r="U50" s="591"/>
-      <c r="V50" s="592"/>
+      <c r="Q50" s="592"/>
+      <c r="R50" s="593"/>
+      <c r="S50" s="593"/>
+      <c r="T50" s="593"/>
+      <c r="U50" s="593"/>
+      <c r="V50" s="594"/>
       <c r="W50" s="565"/>
       <c r="X50" s="566"/>
       <c r="Y50" s="567"/>
@@ -20690,29 +20690,29 @@
       <c r="C51" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D51" s="574"/>
+      <c r="D51" s="587"/>
       <c r="E51" s="575"/>
-      <c r="F51" s="586"/>
-      <c r="G51" s="587"/>
-      <c r="H51" s="587"/>
-      <c r="I51" s="587"/>
-      <c r="J51" s="587"/>
-      <c r="K51" s="587"/>
-      <c r="L51" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M51" s="589" t="s">
+      <c r="F51" s="588"/>
+      <c r="G51" s="589"/>
+      <c r="H51" s="589"/>
+      <c r="I51" s="589"/>
+      <c r="J51" s="589"/>
+      <c r="K51" s="589"/>
+      <c r="L51" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M51" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N51" s="565"/>
       <c r="O51" s="581"/>
       <c r="P51" s="582"/>
-      <c r="Q51" s="590"/>
-      <c r="R51" s="591"/>
-      <c r="S51" s="591"/>
-      <c r="T51" s="591"/>
-      <c r="U51" s="591"/>
-      <c r="V51" s="592"/>
+      <c r="Q51" s="592"/>
+      <c r="R51" s="593"/>
+      <c r="S51" s="593"/>
+      <c r="T51" s="593"/>
+      <c r="U51" s="593"/>
+      <c r="V51" s="594"/>
       <c r="W51" s="565"/>
       <c r="X51" s="566"/>
       <c r="Y51" s="567"/>
@@ -20724,29 +20724,29 @@
       <c r="C52" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D52" s="574"/>
+      <c r="D52" s="587"/>
       <c r="E52" s="575"/>
-      <c r="F52" s="586"/>
-      <c r="G52" s="587"/>
-      <c r="H52" s="587"/>
-      <c r="I52" s="587"/>
-      <c r="J52" s="587"/>
-      <c r="K52" s="587"/>
-      <c r="L52" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M52" s="589" t="s">
+      <c r="F52" s="588"/>
+      <c r="G52" s="589"/>
+      <c r="H52" s="589"/>
+      <c r="I52" s="589"/>
+      <c r="J52" s="589"/>
+      <c r="K52" s="589"/>
+      <c r="L52" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M52" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N52" s="565"/>
       <c r="O52" s="581"/>
       <c r="P52" s="582"/>
-      <c r="Q52" s="590"/>
-      <c r="R52" s="591"/>
-      <c r="S52" s="591"/>
-      <c r="T52" s="591"/>
-      <c r="U52" s="591"/>
-      <c r="V52" s="592"/>
+      <c r="Q52" s="592"/>
+      <c r="R52" s="593"/>
+      <c r="S52" s="593"/>
+      <c r="T52" s="593"/>
+      <c r="U52" s="593"/>
+      <c r="V52" s="594"/>
       <c r="W52" s="565"/>
       <c r="X52" s="566"/>
       <c r="Y52" s="567"/>
@@ -20758,29 +20758,29 @@
       <c r="C53" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D53" s="574"/>
+      <c r="D53" s="587"/>
       <c r="E53" s="575"/>
-      <c r="F53" s="586"/>
-      <c r="G53" s="587"/>
-      <c r="H53" s="587"/>
-      <c r="I53" s="587"/>
-      <c r="J53" s="587"/>
-      <c r="K53" s="587"/>
-      <c r="L53" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M53" s="589" t="s">
+      <c r="F53" s="588"/>
+      <c r="G53" s="589"/>
+      <c r="H53" s="589"/>
+      <c r="I53" s="589"/>
+      <c r="J53" s="589"/>
+      <c r="K53" s="589"/>
+      <c r="L53" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M53" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N53" s="565"/>
       <c r="O53" s="581"/>
       <c r="P53" s="582"/>
-      <c r="Q53" s="590"/>
-      <c r="R53" s="591"/>
-      <c r="S53" s="591"/>
-      <c r="T53" s="591"/>
-      <c r="U53" s="591"/>
-      <c r="V53" s="592"/>
+      <c r="Q53" s="592"/>
+      <c r="R53" s="593"/>
+      <c r="S53" s="593"/>
+      <c r="T53" s="593"/>
+      <c r="U53" s="593"/>
+      <c r="V53" s="594"/>
       <c r="W53" s="565"/>
       <c r="X53" s="566"/>
       <c r="Y53" s="567"/>
@@ -20792,29 +20792,29 @@
       <c r="C54" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D54" s="574"/>
+      <c r="D54" s="587"/>
       <c r="E54" s="575"/>
-      <c r="F54" s="586"/>
-      <c r="G54" s="587"/>
-      <c r="H54" s="587"/>
-      <c r="I54" s="587"/>
-      <c r="J54" s="587"/>
-      <c r="K54" s="587"/>
-      <c r="L54" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M54" s="589" t="s">
+      <c r="F54" s="588"/>
+      <c r="G54" s="589"/>
+      <c r="H54" s="589"/>
+      <c r="I54" s="589"/>
+      <c r="J54" s="589"/>
+      <c r="K54" s="589"/>
+      <c r="L54" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M54" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N54" s="565"/>
       <c r="O54" s="581"/>
       <c r="P54" s="582"/>
-      <c r="Q54" s="590"/>
-      <c r="R54" s="591"/>
-      <c r="S54" s="591"/>
-      <c r="T54" s="591"/>
-      <c r="U54" s="591"/>
-      <c r="V54" s="592"/>
+      <c r="Q54" s="592"/>
+      <c r="R54" s="593"/>
+      <c r="S54" s="593"/>
+      <c r="T54" s="593"/>
+      <c r="U54" s="593"/>
+      <c r="V54" s="594"/>
       <c r="W54" s="565"/>
       <c r="X54" s="566"/>
       <c r="Y54" s="567"/>
@@ -20826,29 +20826,29 @@
       <c r="C55" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D55" s="574"/>
+      <c r="D55" s="587"/>
       <c r="E55" s="575"/>
-      <c r="F55" s="586"/>
-      <c r="G55" s="587"/>
-      <c r="H55" s="587"/>
-      <c r="I55" s="587"/>
-      <c r="J55" s="587"/>
-      <c r="K55" s="587"/>
-      <c r="L55" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M55" s="589" t="s">
+      <c r="F55" s="588"/>
+      <c r="G55" s="589"/>
+      <c r="H55" s="589"/>
+      <c r="I55" s="589"/>
+      <c r="J55" s="589"/>
+      <c r="K55" s="589"/>
+      <c r="L55" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M55" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N55" s="565"/>
       <c r="O55" s="581"/>
       <c r="P55" s="582"/>
-      <c r="Q55" s="590"/>
-      <c r="R55" s="591"/>
-      <c r="S55" s="591"/>
-      <c r="T55" s="591"/>
-      <c r="U55" s="591"/>
-      <c r="V55" s="592"/>
+      <c r="Q55" s="592"/>
+      <c r="R55" s="593"/>
+      <c r="S55" s="593"/>
+      <c r="T55" s="593"/>
+      <c r="U55" s="593"/>
+      <c r="V55" s="594"/>
       <c r="W55" s="565"/>
       <c r="X55" s="566"/>
       <c r="Y55" s="567"/>
@@ -20860,29 +20860,29 @@
       <c r="C56" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D56" s="574"/>
+      <c r="D56" s="587"/>
       <c r="E56" s="575"/>
-      <c r="F56" s="586"/>
-      <c r="G56" s="587"/>
-      <c r="H56" s="587"/>
-      <c r="I56" s="587"/>
-      <c r="J56" s="587"/>
-      <c r="K56" s="587"/>
-      <c r="L56" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M56" s="589" t="s">
+      <c r="F56" s="588"/>
+      <c r="G56" s="589"/>
+      <c r="H56" s="589"/>
+      <c r="I56" s="589"/>
+      <c r="J56" s="589"/>
+      <c r="K56" s="589"/>
+      <c r="L56" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M56" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N56" s="565"/>
       <c r="O56" s="581"/>
       <c r="P56" s="582"/>
-      <c r="Q56" s="590"/>
-      <c r="R56" s="591"/>
-      <c r="S56" s="591"/>
-      <c r="T56" s="591"/>
-      <c r="U56" s="591"/>
-      <c r="V56" s="592"/>
+      <c r="Q56" s="592"/>
+      <c r="R56" s="593"/>
+      <c r="S56" s="593"/>
+      <c r="T56" s="593"/>
+      <c r="U56" s="593"/>
+      <c r="V56" s="594"/>
       <c r="W56" s="565"/>
       <c r="X56" s="566"/>
       <c r="Y56" s="567"/>
@@ -20894,29 +20894,29 @@
       <c r="C57" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D57" s="574"/>
+      <c r="D57" s="587"/>
       <c r="E57" s="575"/>
-      <c r="F57" s="586"/>
-      <c r="G57" s="587"/>
-      <c r="H57" s="587"/>
-      <c r="I57" s="587"/>
-      <c r="J57" s="587"/>
-      <c r="K57" s="587"/>
-      <c r="L57" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M57" s="589" t="s">
+      <c r="F57" s="588"/>
+      <c r="G57" s="589"/>
+      <c r="H57" s="589"/>
+      <c r="I57" s="589"/>
+      <c r="J57" s="589"/>
+      <c r="K57" s="589"/>
+      <c r="L57" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M57" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N57" s="565"/>
       <c r="O57" s="581"/>
       <c r="P57" s="582"/>
-      <c r="Q57" s="590"/>
-      <c r="R57" s="591"/>
-      <c r="S57" s="591"/>
-      <c r="T57" s="591"/>
-      <c r="U57" s="591"/>
-      <c r="V57" s="592"/>
+      <c r="Q57" s="592"/>
+      <c r="R57" s="593"/>
+      <c r="S57" s="593"/>
+      <c r="T57" s="593"/>
+      <c r="U57" s="593"/>
+      <c r="V57" s="594"/>
       <c r="W57" s="565"/>
       <c r="X57" s="566"/>
       <c r="Y57" s="567"/>
@@ -20928,29 +20928,29 @@
       <c r="C58" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D58" s="574"/>
+      <c r="D58" s="587"/>
       <c r="E58" s="575"/>
-      <c r="F58" s="586"/>
-      <c r="G58" s="587"/>
-      <c r="H58" s="587"/>
-      <c r="I58" s="587"/>
-      <c r="J58" s="587"/>
-      <c r="K58" s="587"/>
-      <c r="L58" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M58" s="589" t="s">
+      <c r="F58" s="588"/>
+      <c r="G58" s="589"/>
+      <c r="H58" s="589"/>
+      <c r="I58" s="589"/>
+      <c r="J58" s="589"/>
+      <c r="K58" s="589"/>
+      <c r="L58" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M58" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N58" s="565"/>
       <c r="O58" s="581"/>
       <c r="P58" s="582"/>
-      <c r="Q58" s="590"/>
-      <c r="R58" s="591"/>
-      <c r="S58" s="591"/>
-      <c r="T58" s="591"/>
-      <c r="U58" s="591"/>
-      <c r="V58" s="592"/>
+      <c r="Q58" s="592"/>
+      <c r="R58" s="593"/>
+      <c r="S58" s="593"/>
+      <c r="T58" s="593"/>
+      <c r="U58" s="593"/>
+      <c r="V58" s="594"/>
       <c r="W58" s="565"/>
       <c r="X58" s="566"/>
       <c r="Y58" s="567"/>
@@ -20962,29 +20962,29 @@
       <c r="C59" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D59" s="574"/>
+      <c r="D59" s="587"/>
       <c r="E59" s="575"/>
-      <c r="F59" s="586"/>
-      <c r="G59" s="587"/>
-      <c r="H59" s="587"/>
-      <c r="I59" s="587"/>
-      <c r="J59" s="587"/>
-      <c r="K59" s="587"/>
-      <c r="L59" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M59" s="589" t="s">
+      <c r="F59" s="588"/>
+      <c r="G59" s="589"/>
+      <c r="H59" s="589"/>
+      <c r="I59" s="589"/>
+      <c r="J59" s="589"/>
+      <c r="K59" s="589"/>
+      <c r="L59" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M59" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N59" s="565"/>
       <c r="O59" s="581"/>
       <c r="P59" s="582"/>
-      <c r="Q59" s="590"/>
-      <c r="R59" s="591"/>
-      <c r="S59" s="591"/>
-      <c r="T59" s="591"/>
-      <c r="U59" s="591"/>
-      <c r="V59" s="592"/>
+      <c r="Q59" s="592"/>
+      <c r="R59" s="593"/>
+      <c r="S59" s="593"/>
+      <c r="T59" s="593"/>
+      <c r="U59" s="593"/>
+      <c r="V59" s="594"/>
       <c r="W59" s="565"/>
       <c r="X59" s="566"/>
       <c r="Y59" s="567"/>
@@ -20996,29 +20996,29 @@
       <c r="C60" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D60" s="574"/>
+      <c r="D60" s="587"/>
       <c r="E60" s="575"/>
-      <c r="F60" s="586"/>
-      <c r="G60" s="587"/>
-      <c r="H60" s="587"/>
-      <c r="I60" s="587"/>
-      <c r="J60" s="587"/>
-      <c r="K60" s="587"/>
-      <c r="L60" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M60" s="589" t="s">
+      <c r="F60" s="588"/>
+      <c r="G60" s="589"/>
+      <c r="H60" s="589"/>
+      <c r="I60" s="589"/>
+      <c r="J60" s="589"/>
+      <c r="K60" s="589"/>
+      <c r="L60" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M60" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N60" s="565"/>
       <c r="O60" s="581"/>
       <c r="P60" s="582"/>
-      <c r="Q60" s="590"/>
-      <c r="R60" s="591"/>
-      <c r="S60" s="591"/>
-      <c r="T60" s="591"/>
-      <c r="U60" s="591"/>
-      <c r="V60" s="592"/>
+      <c r="Q60" s="592"/>
+      <c r="R60" s="593"/>
+      <c r="S60" s="593"/>
+      <c r="T60" s="593"/>
+      <c r="U60" s="593"/>
+      <c r="V60" s="594"/>
       <c r="W60" s="565"/>
       <c r="X60" s="566"/>
       <c r="Y60" s="567"/>
@@ -21030,29 +21030,29 @@
       <c r="C61" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D61" s="574"/>
+      <c r="D61" s="587"/>
       <c r="E61" s="575"/>
-      <c r="F61" s="586"/>
-      <c r="G61" s="587"/>
-      <c r="H61" s="587"/>
-      <c r="I61" s="587"/>
-      <c r="J61" s="587"/>
-      <c r="K61" s="587"/>
-      <c r="L61" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M61" s="589" t="s">
+      <c r="F61" s="588"/>
+      <c r="G61" s="589"/>
+      <c r="H61" s="589"/>
+      <c r="I61" s="589"/>
+      <c r="J61" s="589"/>
+      <c r="K61" s="589"/>
+      <c r="L61" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M61" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N61" s="565"/>
       <c r="O61" s="581"/>
       <c r="P61" s="582"/>
-      <c r="Q61" s="590"/>
-      <c r="R61" s="591"/>
-      <c r="S61" s="591"/>
-      <c r="T61" s="591"/>
-      <c r="U61" s="591"/>
-      <c r="V61" s="592"/>
+      <c r="Q61" s="592"/>
+      <c r="R61" s="593"/>
+      <c r="S61" s="593"/>
+      <c r="T61" s="593"/>
+      <c r="U61" s="593"/>
+      <c r="V61" s="594"/>
       <c r="W61" s="565"/>
       <c r="X61" s="566"/>
       <c r="Y61" s="567"/>
@@ -21064,29 +21064,29 @@
       <c r="C62" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D62" s="574"/>
+      <c r="D62" s="587"/>
       <c r="E62" s="575"/>
-      <c r="F62" s="586"/>
-      <c r="G62" s="587"/>
-      <c r="H62" s="587"/>
-      <c r="I62" s="587"/>
-      <c r="J62" s="587"/>
-      <c r="K62" s="587"/>
-      <c r="L62" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M62" s="589" t="s">
+      <c r="F62" s="588"/>
+      <c r="G62" s="589"/>
+      <c r="H62" s="589"/>
+      <c r="I62" s="589"/>
+      <c r="J62" s="589"/>
+      <c r="K62" s="589"/>
+      <c r="L62" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M62" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N62" s="565"/>
       <c r="O62" s="581"/>
       <c r="P62" s="582"/>
-      <c r="Q62" s="590"/>
-      <c r="R62" s="591"/>
-      <c r="S62" s="591"/>
-      <c r="T62" s="591"/>
-      <c r="U62" s="591"/>
-      <c r="V62" s="592"/>
+      <c r="Q62" s="592"/>
+      <c r="R62" s="593"/>
+      <c r="S62" s="593"/>
+      <c r="T62" s="593"/>
+      <c r="U62" s="593"/>
+      <c r="V62" s="594"/>
       <c r="W62" s="565"/>
       <c r="X62" s="566"/>
       <c r="Y62" s="567"/>
@@ -21098,29 +21098,29 @@
       <c r="C63" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D63" s="574"/>
+      <c r="D63" s="587"/>
       <c r="E63" s="575"/>
-      <c r="F63" s="586"/>
-      <c r="G63" s="587"/>
-      <c r="H63" s="587"/>
-      <c r="I63" s="587"/>
-      <c r="J63" s="587"/>
-      <c r="K63" s="587"/>
-      <c r="L63" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M63" s="589" t="s">
+      <c r="F63" s="588"/>
+      <c r="G63" s="589"/>
+      <c r="H63" s="589"/>
+      <c r="I63" s="589"/>
+      <c r="J63" s="589"/>
+      <c r="K63" s="589"/>
+      <c r="L63" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M63" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N63" s="565"/>
       <c r="O63" s="581"/>
       <c r="P63" s="582"/>
-      <c r="Q63" s="590"/>
-      <c r="R63" s="591"/>
-      <c r="S63" s="591"/>
-      <c r="T63" s="591"/>
-      <c r="U63" s="591"/>
-      <c r="V63" s="592"/>
+      <c r="Q63" s="592"/>
+      <c r="R63" s="593"/>
+      <c r="S63" s="593"/>
+      <c r="T63" s="593"/>
+      <c r="U63" s="593"/>
+      <c r="V63" s="594"/>
       <c r="W63" s="565"/>
       <c r="X63" s="566"/>
       <c r="Y63" s="567"/>
@@ -21132,29 +21132,29 @@
       <c r="C64" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D64" s="574"/>
+      <c r="D64" s="587"/>
       <c r="E64" s="575"/>
-      <c r="F64" s="586"/>
-      <c r="G64" s="587"/>
-      <c r="H64" s="587"/>
-      <c r="I64" s="587"/>
-      <c r="J64" s="587"/>
-      <c r="K64" s="587"/>
-      <c r="L64" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M64" s="589" t="s">
+      <c r="F64" s="588"/>
+      <c r="G64" s="589"/>
+      <c r="H64" s="589"/>
+      <c r="I64" s="589"/>
+      <c r="J64" s="589"/>
+      <c r="K64" s="589"/>
+      <c r="L64" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M64" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N64" s="565"/>
       <c r="O64" s="581"/>
       <c r="P64" s="582"/>
-      <c r="Q64" s="590"/>
-      <c r="R64" s="591"/>
-      <c r="S64" s="591"/>
-      <c r="T64" s="591"/>
-      <c r="U64" s="591"/>
-      <c r="V64" s="592"/>
+      <c r="Q64" s="592"/>
+      <c r="R64" s="593"/>
+      <c r="S64" s="593"/>
+      <c r="T64" s="593"/>
+      <c r="U64" s="593"/>
+      <c r="V64" s="594"/>
       <c r="W64" s="565"/>
       <c r="X64" s="566"/>
       <c r="Y64" s="567"/>
@@ -21166,29 +21166,29 @@
       <c r="C65" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D65" s="574"/>
+      <c r="D65" s="587"/>
       <c r="E65" s="575"/>
-      <c r="F65" s="586"/>
-      <c r="G65" s="587"/>
-      <c r="H65" s="587"/>
-      <c r="I65" s="587"/>
-      <c r="J65" s="587"/>
-      <c r="K65" s="587"/>
-      <c r="L65" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M65" s="589" t="s">
+      <c r="F65" s="588"/>
+      <c r="G65" s="589"/>
+      <c r="H65" s="589"/>
+      <c r="I65" s="589"/>
+      <c r="J65" s="589"/>
+      <c r="K65" s="589"/>
+      <c r="L65" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M65" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N65" s="565"/>
       <c r="O65" s="581"/>
       <c r="P65" s="582"/>
-      <c r="Q65" s="590"/>
-      <c r="R65" s="591"/>
-      <c r="S65" s="591"/>
-      <c r="T65" s="591"/>
-      <c r="U65" s="591"/>
-      <c r="V65" s="592"/>
+      <c r="Q65" s="592"/>
+      <c r="R65" s="593"/>
+      <c r="S65" s="593"/>
+      <c r="T65" s="593"/>
+      <c r="U65" s="593"/>
+      <c r="V65" s="594"/>
       <c r="W65" s="565"/>
       <c r="X65" s="566"/>
       <c r="Y65" s="567"/>
@@ -21200,29 +21200,29 @@
       <c r="C66" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D66" s="574"/>
+      <c r="D66" s="587"/>
       <c r="E66" s="575"/>
-      <c r="F66" s="586"/>
-      <c r="G66" s="587"/>
-      <c r="H66" s="587"/>
-      <c r="I66" s="587"/>
-      <c r="J66" s="587"/>
-      <c r="K66" s="587"/>
-      <c r="L66" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M66" s="589" t="s">
+      <c r="F66" s="588"/>
+      <c r="G66" s="589"/>
+      <c r="H66" s="589"/>
+      <c r="I66" s="589"/>
+      <c r="J66" s="589"/>
+      <c r="K66" s="589"/>
+      <c r="L66" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M66" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N66" s="565"/>
       <c r="O66" s="581"/>
       <c r="P66" s="582"/>
-      <c r="Q66" s="590"/>
-      <c r="R66" s="591"/>
-      <c r="S66" s="591"/>
-      <c r="T66" s="591"/>
-      <c r="U66" s="591"/>
-      <c r="V66" s="592"/>
+      <c r="Q66" s="592"/>
+      <c r="R66" s="593"/>
+      <c r="S66" s="593"/>
+      <c r="T66" s="593"/>
+      <c r="U66" s="593"/>
+      <c r="V66" s="594"/>
       <c r="W66" s="565"/>
       <c r="X66" s="566"/>
       <c r="Y66" s="567"/>
@@ -21234,29 +21234,29 @@
       <c r="C67" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D67" s="574"/>
+      <c r="D67" s="587"/>
       <c r="E67" s="575"/>
-      <c r="F67" s="586"/>
-      <c r="G67" s="587"/>
-      <c r="H67" s="587"/>
-      <c r="I67" s="587"/>
-      <c r="J67" s="587"/>
-      <c r="K67" s="587"/>
-      <c r="L67" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M67" s="589" t="s">
+      <c r="F67" s="588"/>
+      <c r="G67" s="589"/>
+      <c r="H67" s="589"/>
+      <c r="I67" s="589"/>
+      <c r="J67" s="589"/>
+      <c r="K67" s="589"/>
+      <c r="L67" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M67" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N67" s="565"/>
       <c r="O67" s="581"/>
       <c r="P67" s="582"/>
-      <c r="Q67" s="590"/>
-      <c r="R67" s="591"/>
-      <c r="S67" s="591"/>
-      <c r="T67" s="591"/>
-      <c r="U67" s="591"/>
-      <c r="V67" s="592"/>
+      <c r="Q67" s="592"/>
+      <c r="R67" s="593"/>
+      <c r="S67" s="593"/>
+      <c r="T67" s="593"/>
+      <c r="U67" s="593"/>
+      <c r="V67" s="594"/>
       <c r="W67" s="565"/>
       <c r="X67" s="566"/>
       <c r="Y67" s="567"/>
@@ -21268,29 +21268,29 @@
       <c r="C68" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D68" s="574"/>
+      <c r="D68" s="587"/>
       <c r="E68" s="575"/>
-      <c r="F68" s="586"/>
-      <c r="G68" s="587"/>
-      <c r="H68" s="587"/>
-      <c r="I68" s="587"/>
-      <c r="J68" s="587"/>
-      <c r="K68" s="587"/>
-      <c r="L68" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M68" s="589" t="s">
+      <c r="F68" s="588"/>
+      <c r="G68" s="589"/>
+      <c r="H68" s="589"/>
+      <c r="I68" s="589"/>
+      <c r="J68" s="589"/>
+      <c r="K68" s="589"/>
+      <c r="L68" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M68" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N68" s="565"/>
       <c r="O68" s="581"/>
       <c r="P68" s="582"/>
-      <c r="Q68" s="590"/>
-      <c r="R68" s="591"/>
-      <c r="S68" s="591"/>
-      <c r="T68" s="591"/>
-      <c r="U68" s="591"/>
-      <c r="V68" s="592"/>
+      <c r="Q68" s="592"/>
+      <c r="R68" s="593"/>
+      <c r="S68" s="593"/>
+      <c r="T68" s="593"/>
+      <c r="U68" s="593"/>
+      <c r="V68" s="594"/>
       <c r="W68" s="565"/>
       <c r="X68" s="566"/>
       <c r="Y68" s="567"/>
@@ -21302,29 +21302,29 @@
       <c r="C69" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D69" s="574"/>
+      <c r="D69" s="587"/>
       <c r="E69" s="575"/>
-      <c r="F69" s="586"/>
-      <c r="G69" s="587"/>
-      <c r="H69" s="587"/>
-      <c r="I69" s="587"/>
-      <c r="J69" s="587"/>
-      <c r="K69" s="587"/>
-      <c r="L69" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M69" s="589" t="s">
+      <c r="F69" s="588"/>
+      <c r="G69" s="589"/>
+      <c r="H69" s="589"/>
+      <c r="I69" s="589"/>
+      <c r="J69" s="589"/>
+      <c r="K69" s="589"/>
+      <c r="L69" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M69" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N69" s="565"/>
       <c r="O69" s="581"/>
       <c r="P69" s="582"/>
-      <c r="Q69" s="590"/>
-      <c r="R69" s="591"/>
-      <c r="S69" s="591"/>
-      <c r="T69" s="591"/>
-      <c r="U69" s="591"/>
-      <c r="V69" s="592"/>
+      <c r="Q69" s="592"/>
+      <c r="R69" s="593"/>
+      <c r="S69" s="593"/>
+      <c r="T69" s="593"/>
+      <c r="U69" s="593"/>
+      <c r="V69" s="594"/>
       <c r="W69" s="565"/>
       <c r="X69" s="566"/>
       <c r="Y69" s="567"/>
@@ -21336,29 +21336,29 @@
       <c r="C70" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D70" s="574"/>
+      <c r="D70" s="587"/>
       <c r="E70" s="575"/>
-      <c r="F70" s="586"/>
-      <c r="G70" s="587"/>
-      <c r="H70" s="587"/>
-      <c r="I70" s="587"/>
-      <c r="J70" s="587"/>
-      <c r="K70" s="587"/>
-      <c r="L70" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M70" s="589" t="s">
+      <c r="F70" s="588"/>
+      <c r="G70" s="589"/>
+      <c r="H70" s="589"/>
+      <c r="I70" s="589"/>
+      <c r="J70" s="589"/>
+      <c r="K70" s="589"/>
+      <c r="L70" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M70" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N70" s="565"/>
       <c r="O70" s="581"/>
       <c r="P70" s="582"/>
-      <c r="Q70" s="590"/>
-      <c r="R70" s="591"/>
-      <c r="S70" s="591"/>
-      <c r="T70" s="591"/>
-      <c r="U70" s="591"/>
-      <c r="V70" s="592"/>
+      <c r="Q70" s="592"/>
+      <c r="R70" s="593"/>
+      <c r="S70" s="593"/>
+      <c r="T70" s="593"/>
+      <c r="U70" s="593"/>
+      <c r="V70" s="594"/>
       <c r="W70" s="565"/>
       <c r="X70" s="566"/>
       <c r="Y70" s="567"/>
@@ -21370,29 +21370,29 @@
       <c r="C71" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D71" s="574"/>
+      <c r="D71" s="587"/>
       <c r="E71" s="575"/>
-      <c r="F71" s="586"/>
-      <c r="G71" s="587"/>
-      <c r="H71" s="587"/>
-      <c r="I71" s="587"/>
-      <c r="J71" s="587"/>
-      <c r="K71" s="587"/>
-      <c r="L71" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M71" s="589" t="s">
+      <c r="F71" s="588"/>
+      <c r="G71" s="589"/>
+      <c r="H71" s="589"/>
+      <c r="I71" s="589"/>
+      <c r="J71" s="589"/>
+      <c r="K71" s="589"/>
+      <c r="L71" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M71" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N71" s="565"/>
       <c r="O71" s="581"/>
       <c r="P71" s="582"/>
-      <c r="Q71" s="590"/>
-      <c r="R71" s="591"/>
-      <c r="S71" s="591"/>
-      <c r="T71" s="591"/>
-      <c r="U71" s="591"/>
-      <c r="V71" s="592"/>
+      <c r="Q71" s="592"/>
+      <c r="R71" s="593"/>
+      <c r="S71" s="593"/>
+      <c r="T71" s="593"/>
+      <c r="U71" s="593"/>
+      <c r="V71" s="594"/>
       <c r="W71" s="565"/>
       <c r="X71" s="566"/>
       <c r="Y71" s="567"/>
@@ -21404,32 +21404,32 @@
       <c r="C72" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D72" s="574"/>
+      <c r="D72" s="587"/>
       <c r="E72" s="575"/>
-      <c r="F72" s="586"/>
-      <c r="G72" s="587"/>
-      <c r="H72" s="587"/>
-      <c r="I72" s="587"/>
-      <c r="J72" s="587"/>
-      <c r="K72" s="587"/>
-      <c r="L72" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M72" s="589" t="s">
+      <c r="F72" s="588"/>
+      <c r="G72" s="589"/>
+      <c r="H72" s="589"/>
+      <c r="I72" s="589"/>
+      <c r="J72" s="589"/>
+      <c r="K72" s="589"/>
+      <c r="L72" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M72" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N72" s="565"/>
       <c r="O72" s="581"/>
       <c r="P72" s="582"/>
-      <c r="Q72" s="590"/>
-      <c r="R72" s="595"/>
-      <c r="S72" s="595"/>
-      <c r="T72" s="595"/>
-      <c r="U72" s="595"/>
-      <c r="V72" s="595"/>
-      <c r="W72" s="596"/>
-      <c r="X72" s="597"/>
-      <c r="Y72" s="598"/>
+      <c r="Q72" s="592"/>
+      <c r="R72" s="597"/>
+      <c r="S72" s="597"/>
+      <c r="T72" s="597"/>
+      <c r="U72" s="597"/>
+      <c r="V72" s="597"/>
+      <c r="W72" s="598"/>
+      <c r="X72" s="599"/>
+      <c r="Y72" s="600"/>
     </row>
     <row r="73" spans="2:40" ht="42" customHeight="1">
       <c r="B73" s="572">
@@ -21438,32 +21438,32 @@
       <c r="C73" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D73" s="574"/>
+      <c r="D73" s="587"/>
       <c r="E73" s="575"/>
-      <c r="F73" s="586"/>
-      <c r="G73" s="587"/>
-      <c r="H73" s="587"/>
-      <c r="I73" s="587"/>
-      <c r="J73" s="587"/>
-      <c r="K73" s="587"/>
-      <c r="L73" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M73" s="589" t="s">
+      <c r="F73" s="588"/>
+      <c r="G73" s="589"/>
+      <c r="H73" s="589"/>
+      <c r="I73" s="589"/>
+      <c r="J73" s="589"/>
+      <c r="K73" s="589"/>
+      <c r="L73" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M73" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N73" s="565"/>
       <c r="O73" s="581"/>
       <c r="P73" s="582"/>
-      <c r="Q73" s="590"/>
-      <c r="R73" s="599"/>
-      <c r="S73" s="599"/>
-      <c r="T73" s="599"/>
-      <c r="U73" s="599"/>
-      <c r="V73" s="599"/>
-      <c r="W73" s="599"/>
-      <c r="X73" s="599"/>
-      <c r="Y73" s="600"/>
+      <c r="Q73" s="592"/>
+      <c r="R73" s="601"/>
+      <c r="S73" s="601"/>
+      <c r="T73" s="601"/>
+      <c r="U73" s="601"/>
+      <c r="V73" s="601"/>
+      <c r="W73" s="601"/>
+      <c r="X73" s="601"/>
+      <c r="Y73" s="602"/>
     </row>
     <row r="74" spans="2:40" ht="42" customHeight="1">
       <c r="B74" s="572">
@@ -21472,32 +21472,32 @@
       <c r="C74" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D74" s="574"/>
+      <c r="D74" s="587"/>
       <c r="E74" s="575"/>
-      <c r="F74" s="586"/>
-      <c r="G74" s="587"/>
-      <c r="H74" s="587"/>
-      <c r="I74" s="587"/>
-      <c r="J74" s="587"/>
-      <c r="K74" s="587"/>
-      <c r="L74" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M74" s="589" t="s">
+      <c r="F74" s="588"/>
+      <c r="G74" s="589"/>
+      <c r="H74" s="589"/>
+      <c r="I74" s="589"/>
+      <c r="J74" s="589"/>
+      <c r="K74" s="589"/>
+      <c r="L74" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M74" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N74" s="565"/>
       <c r="O74" s="581"/>
       <c r="P74" s="582"/>
-      <c r="Q74" s="590"/>
-      <c r="R74" s="601"/>
-      <c r="S74" s="601"/>
-      <c r="T74" s="601"/>
-      <c r="U74" s="601"/>
-      <c r="V74" s="601"/>
-      <c r="W74" s="601"/>
-      <c r="X74" s="601"/>
-      <c r="Y74" s="602"/>
+      <c r="Q74" s="592"/>
+      <c r="R74" s="603"/>
+      <c r="S74" s="603"/>
+      <c r="T74" s="603"/>
+      <c r="U74" s="603"/>
+      <c r="V74" s="603"/>
+      <c r="W74" s="603"/>
+      <c r="X74" s="603"/>
+      <c r="Y74" s="604"/>
     </row>
     <row r="75" spans="2:40" ht="42" customHeight="1">
       <c r="B75" s="572">
@@ -21506,32 +21506,32 @@
       <c r="C75" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D75" s="574"/>
+      <c r="D75" s="587"/>
       <c r="E75" s="575"/>
-      <c r="F75" s="586"/>
-      <c r="G75" s="587"/>
-      <c r="H75" s="587"/>
-      <c r="I75" s="587"/>
-      <c r="J75" s="587"/>
-      <c r="K75" s="587"/>
-      <c r="L75" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M75" s="589" t="s">
+      <c r="F75" s="588"/>
+      <c r="G75" s="589"/>
+      <c r="H75" s="589"/>
+      <c r="I75" s="589"/>
+      <c r="J75" s="589"/>
+      <c r="K75" s="589"/>
+      <c r="L75" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M75" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N75" s="565"/>
       <c r="O75" s="581"/>
       <c r="P75" s="582"/>
-      <c r="Q75" s="590"/>
-      <c r="R75" s="603"/>
-      <c r="S75" s="603"/>
-      <c r="T75" s="603"/>
-      <c r="U75" s="603"/>
-      <c r="V75" s="603"/>
-      <c r="W75" s="603"/>
-      <c r="X75" s="603"/>
-      <c r="Y75" s="604"/>
+      <c r="Q75" s="592"/>
+      <c r="R75" s="605"/>
+      <c r="S75" s="605"/>
+      <c r="T75" s="605"/>
+      <c r="U75" s="605"/>
+      <c r="V75" s="605"/>
+      <c r="W75" s="605"/>
+      <c r="X75" s="605"/>
+      <c r="Y75" s="606"/>
     </row>
     <row r="76" spans="2:40" ht="42" customHeight="1">
       <c r="B76" s="572">
@@ -21540,32 +21540,32 @@
       <c r="C76" s="573" t="s">
         <v>60</v>
       </c>
-      <c r="D76" s="574"/>
+      <c r="D76" s="587"/>
       <c r="E76" s="575"/>
-      <c r="F76" s="586"/>
-      <c r="G76" s="587"/>
-      <c r="H76" s="587"/>
-      <c r="I76" s="587"/>
-      <c r="J76" s="587"/>
-      <c r="K76" s="587"/>
-      <c r="L76" s="588" t="s">
-        <v>60</v>
-      </c>
-      <c r="M76" s="589" t="s">
+      <c r="F76" s="588"/>
+      <c r="G76" s="589"/>
+      <c r="H76" s="589"/>
+      <c r="I76" s="589"/>
+      <c r="J76" s="589"/>
+      <c r="K76" s="589"/>
+      <c r="L76" s="590" t="s">
+        <v>60</v>
+      </c>
+      <c r="M76" s="591" t="s">
         <v>60</v>
       </c>
       <c r="N76" s="565"/>
       <c r="O76" s="581"/>
       <c r="P76" s="582"/>
-      <c r="Q76" s="590"/>
-      <c r="R76" s="605"/>
-      <c r="S76" s="605"/>
-      <c r="T76" s="605"/>
-      <c r="U76" s="605"/>
-      <c r="V76" s="605"/>
-      <c r="W76" s="605"/>
-      <c r="X76" s="605"/>
-      <c r="Y76" s="606"/>
+      <c r="Q76" s="592"/>
+      <c r="R76" s="607"/>
+      <c r="S76" s="607"/>
+      <c r="T76" s="607"/>
+      <c r="U76" s="607"/>
+      <c r="V76" s="607"/>
+      <c r="W76" s="607"/>
+      <c r="X76" s="607"/>
+      <c r="Y76" s="608"/>
     </row>
     <row r="77" spans="2:40">
       <c r="AN77" s="456"/>
@@ -21597,6 +21597,7 @@
     <mergeCell ref="Q28:V28"/>
     <mergeCell ref="F28:K28"/>
     <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Q32:V32"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="T1:Y1"/>
     <mergeCell ref="G3:I3"/>
@@ -21620,6 +21621,7 @@
     <mergeCell ref="J5:O6"/>
     <mergeCell ref="J8:O8"/>
     <mergeCell ref="J10:O10"/>
+    <mergeCell ref="G10:I10"/>
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="L16:M16"/>
     <mergeCell ref="N16:O16"/>
@@ -21632,7 +21634,6 @@
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="R17:T17"/>
-    <mergeCell ref="G10:I10"/>
     <mergeCell ref="U17:W17"/>
     <mergeCell ref="X18:Y18"/>
     <mergeCell ref="B23:C23"/>
@@ -21742,6 +21743,7 @@
     <mergeCell ref="O45:P45"/>
     <mergeCell ref="X52:Y52"/>
     <mergeCell ref="X48:Y48"/>
+    <mergeCell ref="X50:Y50"/>
     <mergeCell ref="X42:Y42"/>
     <mergeCell ref="F46:K46"/>
     <mergeCell ref="O46:P46"/>
@@ -21766,10 +21768,6 @@
     <mergeCell ref="O40:P40"/>
     <mergeCell ref="X43:Y43"/>
     <mergeCell ref="X41:Y41"/>
-    <mergeCell ref="X50:Y50"/>
-    <mergeCell ref="F56:K56"/>
-    <mergeCell ref="O56:P56"/>
-    <mergeCell ref="O55:P55"/>
     <mergeCell ref="F47:K47"/>
     <mergeCell ref="O47:P47"/>
     <mergeCell ref="X47:Y47"/>
@@ -21780,10 +21778,7 @@
     <mergeCell ref="X49:Y49"/>
     <mergeCell ref="F55:K55"/>
     <mergeCell ref="X55:Y55"/>
-    <mergeCell ref="X56:Y56"/>
     <mergeCell ref="X53:Y53"/>
-    <mergeCell ref="F59:K59"/>
-    <mergeCell ref="O59:P59"/>
     <mergeCell ref="X54:Y54"/>
     <mergeCell ref="O57:P57"/>
     <mergeCell ref="F57:K57"/>
@@ -21791,8 +21786,10 @@
     <mergeCell ref="O53:P53"/>
     <mergeCell ref="F53:K53"/>
     <mergeCell ref="X60:Y60"/>
-    <mergeCell ref="F62:K62"/>
-    <mergeCell ref="O62:P62"/>
+    <mergeCell ref="F56:K56"/>
+    <mergeCell ref="O56:P56"/>
+    <mergeCell ref="O55:P55"/>
+    <mergeCell ref="X56:Y56"/>
     <mergeCell ref="X57:Y57"/>
     <mergeCell ref="F63:K63"/>
     <mergeCell ref="O63:P63"/>
@@ -21803,7 +21800,8 @@
     <mergeCell ref="O61:P61"/>
     <mergeCell ref="F58:K58"/>
     <mergeCell ref="O58:P58"/>
-    <mergeCell ref="X64:Y64"/>
+    <mergeCell ref="F59:K59"/>
+    <mergeCell ref="O59:P59"/>
     <mergeCell ref="F66:K66"/>
     <mergeCell ref="O66:P66"/>
     <mergeCell ref="X61:Y61"/>
@@ -21818,7 +21816,8 @@
     <mergeCell ref="O64:P64"/>
     <mergeCell ref="F65:K65"/>
     <mergeCell ref="O65:P65"/>
-    <mergeCell ref="Q32:V32"/>
+    <mergeCell ref="F62:K62"/>
+    <mergeCell ref="O62:P62"/>
     <mergeCell ref="Q33:V33"/>
     <mergeCell ref="F76:K76"/>
     <mergeCell ref="O76:P76"/>
@@ -21842,6 +21841,7 @@
     <mergeCell ref="X63:Y63"/>
     <mergeCell ref="F69:K69"/>
     <mergeCell ref="O69:P69"/>
+    <mergeCell ref="X64:Y64"/>
   </mergeCells>
   <phoneticPr fontId="6"/>
   <conditionalFormatting sqref="H16:I16 L16:M16 P16:Q16 H17 F18">

</xml_diff>